<commit_message>
plot scores relative to all core ; plot tree ; first core files
</commit_message>
<xml_diff>
--- a/webapp/llm_extensions/prompts.xlsx
+++ b/webapp/llm_extensions/prompts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\llmSparklis\webapp\llm_extensions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43F3C7C-7574-46CA-B5C1-9B1AA63D97DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5687F928-4C4B-4227-BF94-B5610807F866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{B16B8F13-8ED3-4425-9032-2DAF56525750}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{B16B8F13-8ED3-4425-9032-2DAF56525750}"/>
   </bookViews>
   <sheets>
     <sheet name="llm_extension_with_qa_extension" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Remarques</t>
   </si>
@@ -409,6 +409,21 @@
 A: I can start by finding FOUNDERS of something called TENCENT. Then, I can filter by people who have been members of the NATIONAL PEOPLE'S CONGRESS.
 &lt;commands&gt;backwardProperty founder of ; Tencent ; forwardProperty position ; National People's Congress&lt;/commands&gt;
 `;</t>
+  </si>
+  <si>
+    <t>kill bill vol 1</t>
+  </si>
+  <si>
+    <t>Filter "publication"</t>
+  </si>
+  <si>
+    <t>selectionne seul résultat</t>
+  </si>
+  <si>
+    <t>after 2004</t>
+  </si>
+  <si>
+    <t>post traitement compter</t>
   </si>
 </sst>
 </file>
@@ -785,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5BFFB1-2617-49CC-A9B0-5B0B9A5D82B2}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -979,10 +994,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84461D4D-A47F-4FB2-8BD4-5B412FAAB0C4}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,9 +1006,10 @@
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="59.5703125" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1004,7 +1020,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1016,6 +1032,23 @@
       </c>
       <c r="D2" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
direct sparql ; new prompts ; details
</commit_message>
<xml_diff>
--- a/webapp/llm_extensions/prompts.xlsx
+++ b/webapp/llm_extensions/prompts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\llmSparklis\webapp\llm_extensions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5687F928-4C4B-4227-BF94-B5610807F866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4CC164-7907-4B31-A0C6-105F03E8259A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{B16B8F13-8ED3-4425-9032-2DAF56525750}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{B16B8F13-8ED3-4425-9032-2DAF56525750}"/>
   </bookViews>
   <sheets>
     <sheet name="llm_extension_with_qa_extension" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Remarques</t>
   </si>
@@ -424,6 +424,41 @@
   </si>
   <si>
     <t>post traitement compter</t>
+  </si>
+  <si>
+    <t>`
+    ## Task: Generate knowledge graph query commands for Sparklis.
+    ## Format:  
+    1. Think step by step about what entities and relationships are needed 
+    2. Then finish your response by a list of commands, separated by semicolons (;), and wrapped in &lt;commands&gt;...&lt;/commands&gt;.  
+    ### Available Commands:
+    - a [concept] → Retrieve entities of a given concept (e.g., "a book" to find books).
+    - [entity] → Retrieve an entity (e.g., "Albert Einstein" to find the entity representing Einstein).
+    - forwardProperty [property] → Filter by property (e.g., "forwardProperty director" to find films directed by someone).
+    - backwardProperty [property] → Reverse relation (e.g., "backwardProperty director" to find directors of films).
+    - higherThan [number], lowerThan [number] → Value constraints.
+    - after [date], before [date] → Time constraints.  
+    - and, or → Logical operators.  
+    ## Examples:
+    Q: At which school went Yayoi Kusama?
+    A: Starting from the list of entities named Yayoi Kusama seems the best approach. Then, I just need to find the relationship that represents at which school she was educated.
+    &lt;commands&gt;Yayoi Kusama ; forwardProperty educated at&lt;/commands&gt; 
+    Q: What is the boiling point of water?
+    A: The core of the request is WATER. From this entity I will probably be able to get a property such as its BOILING POINT.  
+    &lt;commands&gt;water; forwardProperty boiling point&lt;/commands&gt;  
+    Q: Movies by Spielberg or Tim Burton after 1980?
+    A: I need to find FILMS by Spielberg or Burton released after 1980. I can start by listing FILMS and then filter by DIRECTOR and RELEASE DATE. 
+    &lt;commands&gt;a film; forwardProperty director; Tim Burton; or; Spielberg; forwardProperty release date; after 1980&lt;/commands&gt;  
+    Q: among the founders of tencent company, who has been member of national people' congress?"
+    A: I can start by finding FOUNDERS of something called TENCENT. Then, I can filter by people who have been members of the NATIONAL PEOPLE'S CONGRESS.
+    &lt;commands&gt;backwardProperty founder of; Tencent ; forwardProperty position ; National People's Congress&lt;/commands&gt;
+    `</t>
+  </si>
+  <si>
+    <t>patch backward</t>
+  </si>
+  <si>
+    <t>v10</t>
   </si>
 </sst>
 </file>
@@ -798,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5BFFB1-2617-49CC-A9B0-5B0B9A5D82B2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,6 +937,17 @@
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84461D4D-A47F-4FB2-8BD4-5B412FAAB0C4}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>